<commit_message>
In the middle of testing kmeans algorithms
</commit_message>
<xml_diff>
--- a/data/01_raw/Ergonautus/Ergonautus_Clusters_Correct_Values.xlsx
+++ b/data/01_raw/Ergonautus/Ergonautus_Clusters_Correct_Values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryerrabelli/Library/CloudStorage/GoogleDrive-ryerrabelli@gmail.com/My Drive/Computer Backups/Rahul Yerrabelli drive/PythonProjects/EyeTraumaAnalysis/data/01_raw/Ergonautus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97406260-B55A-4EC7-96FB-CECCD5289090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE78201C-030C-C144-82B5-ACC2CC22E581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F01288D-5119-41AE-A008-8C44E550E9EF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{1F01288D-5119-41AE-A008-8C44E550E9EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>File Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Correct 1</t>
   </si>
@@ -50,9 +47,6 @@
     <t>Correct 3</t>
   </si>
   <si>
-    <t>Not Ideal</t>
-  </si>
-  <si>
     <t>*note: this entire image is not ideal</t>
   </si>
   <si>
@@ -66,6 +60,450 @@
   </si>
   <si>
     <t>*note: entire image not ideal; lots of skin in image</t>
+  </si>
+  <si>
+    <t>Borderline</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>14000.png</t>
+  </si>
+  <si>
+    <t>14001.png</t>
+  </si>
+  <si>
+    <t>14002.png</t>
+  </si>
+  <si>
+    <t>14003.png</t>
+  </si>
+  <si>
+    <t>14004.png</t>
+  </si>
+  <si>
+    <t>14005.png</t>
+  </si>
+  <si>
+    <t>14006.png</t>
+  </si>
+  <si>
+    <t>14007.png</t>
+  </si>
+  <si>
+    <t>14008.png</t>
+  </si>
+  <si>
+    <t>14009.png</t>
+  </si>
+  <si>
+    <t>14010.png</t>
+  </si>
+  <si>
+    <t>14011.png</t>
+  </si>
+  <si>
+    <t>14012.png</t>
+  </si>
+  <si>
+    <t>14013.png</t>
+  </si>
+  <si>
+    <t>14014.png</t>
+  </si>
+  <si>
+    <t>14015.png</t>
+  </si>
+  <si>
+    <t>14016.png</t>
+  </si>
+  <si>
+    <t>14017.png</t>
+  </si>
+  <si>
+    <t>14018.png</t>
+  </si>
+  <si>
+    <t>14019.png</t>
+  </si>
+  <si>
+    <t>14020.png</t>
+  </si>
+  <si>
+    <t>14021.png</t>
+  </si>
+  <si>
+    <t>14022.png</t>
+  </si>
+  <si>
+    <t>14023.png</t>
+  </si>
+  <si>
+    <t>14024.png</t>
+  </si>
+  <si>
+    <t>14025.png</t>
+  </si>
+  <si>
+    <t>14026.png</t>
+  </si>
+  <si>
+    <t>14104.png</t>
+  </si>
+  <si>
+    <t>14105.png</t>
+  </si>
+  <si>
+    <t>14106.png</t>
+  </si>
+  <si>
+    <t>14107.png</t>
+  </si>
+  <si>
+    <t>14108.png</t>
+  </si>
+  <si>
+    <t>14109.png</t>
+  </si>
+  <si>
+    <t>14110.png</t>
+  </si>
+  <si>
+    <t>14111.png</t>
+  </si>
+  <si>
+    <t>14112.png</t>
+  </si>
+  <si>
+    <t>14113.png</t>
+  </si>
+  <si>
+    <t>14114.png</t>
+  </si>
+  <si>
+    <t>14115.png</t>
+  </si>
+  <si>
+    <t>14116.png</t>
+  </si>
+  <si>
+    <t>14117.png</t>
+  </si>
+  <si>
+    <t>14118.png</t>
+  </si>
+  <si>
+    <t>14119.png</t>
+  </si>
+  <si>
+    <t>14120.png</t>
+  </si>
+  <si>
+    <t>14121.png</t>
+  </si>
+  <si>
+    <t>14122.png</t>
+  </si>
+  <si>
+    <t>14123.png</t>
+  </si>
+  <si>
+    <t>14124.png</t>
+  </si>
+  <si>
+    <t>14125.png</t>
+  </si>
+  <si>
+    <t>14126.png</t>
+  </si>
+  <si>
+    <t>14127.png</t>
+  </si>
+  <si>
+    <t>14128.png</t>
+  </si>
+  <si>
+    <t>14129.png</t>
+  </si>
+  <si>
+    <t>14130.png</t>
+  </si>
+  <si>
+    <t>14131.png</t>
+  </si>
+  <si>
+    <t>14132.png</t>
+  </si>
+  <si>
+    <t>14133.png</t>
+  </si>
+  <si>
+    <t>14134.png</t>
+  </si>
+  <si>
+    <t>14135.png</t>
+  </si>
+  <si>
+    <t>14136.png</t>
+  </si>
+  <si>
+    <t>14137.png</t>
+  </si>
+  <si>
+    <t>14138.png</t>
+  </si>
+  <si>
+    <t>14139.png</t>
+  </si>
+  <si>
+    <t>14140.png</t>
+  </si>
+  <si>
+    <t>14141.png</t>
+  </si>
+  <si>
+    <t>14142.png</t>
+  </si>
+  <si>
+    <t>14143.png</t>
+  </si>
+  <si>
+    <t>14144.png</t>
+  </si>
+  <si>
+    <t>14145.png</t>
+  </si>
+  <si>
+    <t>14146.png</t>
+  </si>
+  <si>
+    <t>14147.png</t>
+  </si>
+  <si>
+    <t>14148.png</t>
+  </si>
+  <si>
+    <t>14149.png</t>
+  </si>
+  <si>
+    <t>14290.png</t>
+  </si>
+  <si>
+    <t>14291.png</t>
+  </si>
+  <si>
+    <t>14292.png</t>
+  </si>
+  <si>
+    <t>14293.png</t>
+  </si>
+  <si>
+    <t>14294.png</t>
+  </si>
+  <si>
+    <t>14295.png</t>
+  </si>
+  <si>
+    <t>14296.png</t>
+  </si>
+  <si>
+    <t>14297.png</t>
+  </si>
+  <si>
+    <t>14298.png</t>
+  </si>
+  <si>
+    <t>14299.png</t>
+  </si>
+  <si>
+    <t>14300.png</t>
+  </si>
+  <si>
+    <t>14301.png</t>
+  </si>
+  <si>
+    <t>14302.png</t>
+  </si>
+  <si>
+    <t>14303.png</t>
+  </si>
+  <si>
+    <t>14304.png</t>
+  </si>
+  <si>
+    <t>14305.png</t>
+  </si>
+  <si>
+    <t>14306.png</t>
+  </si>
+  <si>
+    <t>14307.png</t>
+  </si>
+  <si>
+    <t>14308.png</t>
+  </si>
+  <si>
+    <t>14309.png</t>
+  </si>
+  <si>
+    <t>14310.png</t>
+  </si>
+  <si>
+    <t>14311.png</t>
+  </si>
+  <si>
+    <t>14312.png</t>
+  </si>
+  <si>
+    <t>14313.png</t>
+  </si>
+  <si>
+    <t>14314.png</t>
+  </si>
+  <si>
+    <t>14315.png</t>
+  </si>
+  <si>
+    <t>14394.png</t>
+  </si>
+  <si>
+    <t>14395.png</t>
+  </si>
+  <si>
+    <t>14396.png</t>
+  </si>
+  <si>
+    <t>14397.png</t>
+  </si>
+  <si>
+    <t>14398.png</t>
+  </si>
+  <si>
+    <t>14399.png</t>
+  </si>
+  <si>
+    <t>14400.png</t>
+  </si>
+  <si>
+    <t>14401.png</t>
+  </si>
+  <si>
+    <t>14402.png</t>
+  </si>
+  <si>
+    <t>14403.png</t>
+  </si>
+  <si>
+    <t>14404.png</t>
+  </si>
+  <si>
+    <t>14405.png</t>
+  </si>
+  <si>
+    <t>14406.png</t>
+  </si>
+  <si>
+    <t>14407.png</t>
+  </si>
+  <si>
+    <t>14408.png</t>
+  </si>
+  <si>
+    <t>14409.png</t>
+  </si>
+  <si>
+    <t>14410.png</t>
+  </si>
+  <si>
+    <t>14411.png</t>
+  </si>
+  <si>
+    <t>14412.png</t>
+  </si>
+  <si>
+    <t>14413.png</t>
+  </si>
+  <si>
+    <t>14414.png</t>
+  </si>
+  <si>
+    <t>14415.png</t>
+  </si>
+  <si>
+    <t>14416.png</t>
+  </si>
+  <si>
+    <t>14417.png</t>
+  </si>
+  <si>
+    <t>14418.png</t>
+  </si>
+  <si>
+    <t>14419.png</t>
+  </si>
+  <si>
+    <t>14420.png</t>
+  </si>
+  <si>
+    <t>14421.png</t>
+  </si>
+  <si>
+    <t>14422.png</t>
+  </si>
+  <si>
+    <t>14423.png</t>
+  </si>
+  <si>
+    <t>14424.png</t>
+  </si>
+  <si>
+    <t>14425.png</t>
+  </si>
+  <si>
+    <t>14426.png</t>
+  </si>
+  <si>
+    <t>14427.png</t>
+  </si>
+  <si>
+    <t>14428.png</t>
+  </si>
+  <si>
+    <t>14429.png</t>
+  </si>
+  <si>
+    <t>14430.png</t>
+  </si>
+  <si>
+    <t>14431.png</t>
+  </si>
+  <si>
+    <t>14432.png</t>
+  </si>
+  <si>
+    <t>14433.png</t>
+  </si>
+  <si>
+    <t>14434.png</t>
+  </si>
+  <si>
+    <t>14435.png</t>
+  </si>
+  <si>
+    <t>14436.png</t>
+  </si>
+  <si>
+    <t>14437.png</t>
+  </si>
+  <si>
+    <t>14438.png</t>
+  </si>
+  <si>
+    <t>14439.png</t>
+  </si>
+  <si>
+    <t>Filename</t>
   </si>
 </sst>
 </file>
@@ -109,10 +547,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,35 +866,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E03BA4D-B119-4C1E-B7FD-04F65F29F553}">
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="H143" sqref="H143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>14000</v>
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -466,9 +908,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>14001</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -477,9 +919,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>14002</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -491,9 +933,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>14003</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -505,9 +947,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>14004</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -516,9 +958,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>14005</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -527,9 +969,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>14006</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -538,9 +980,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>14007</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -549,9 +991,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>14008</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -560,9 +1002,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>14009</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -571,9 +1013,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>14010</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -582,9 +1024,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>14011</v>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -593,9 +1035,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>14012</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -607,9 +1049,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14013</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -618,9 +1060,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>14014</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -629,9 +1071,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>14015</v>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -643,17 +1085,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>14016</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>14017</v>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -662,9 +1104,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>14018</v>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -673,9 +1115,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>14019</v>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -684,9 +1126,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>14020</v>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
       </c>
       <c r="B22">
         <v>9</v>
@@ -695,9 +1137,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>14021</v>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
       </c>
       <c r="B23">
         <v>9</v>
@@ -706,9 +1148,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>14022</v>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -717,17 +1159,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>14023</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>14024</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -736,9 +1178,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>14025</v>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -747,9 +1189,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>14026</v>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -761,9 +1203,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>14104</v>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
       </c>
       <c r="B29">
         <v>9</v>
@@ -772,9 +1214,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>14105</v>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -783,9 +1225,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>14106</v>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -794,12 +1236,12 @@
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>14107</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>40</v>
       </c>
       <c r="B32">
         <v>9</v>
@@ -808,9 +1250,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>14108</v>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -819,9 +1261,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>14109</v>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>42</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -830,25 +1272,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>14110</v>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>43</v>
       </c>
       <c r="B35">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>14111</v>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>44</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>14112</v>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -857,9 +1299,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>14113</v>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>46</v>
       </c>
       <c r="B38">
         <v>9</v>
@@ -868,9 +1310,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>14114</v>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>47</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -879,9 +1321,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>14115</v>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -890,9 +1332,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>14116</v>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>49</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -901,9 +1343,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>14117</v>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>50</v>
       </c>
       <c r="B42">
         <v>8</v>
@@ -912,9 +1354,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>14118</v>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>51</v>
       </c>
       <c r="B43">
         <v>9</v>
@@ -923,9 +1365,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>14119</v>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>52</v>
       </c>
       <c r="B44">
         <v>9</v>
@@ -934,17 +1376,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>14120</v>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>53</v>
       </c>
       <c r="B45">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>14121</v>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>54</v>
       </c>
       <c r="B46">
         <v>9</v>
@@ -953,9 +1395,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>14122</v>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>55</v>
       </c>
       <c r="B47">
         <v>10</v>
@@ -964,17 +1406,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>14123</v>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>56</v>
       </c>
       <c r="B48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>14124</v>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>57</v>
       </c>
       <c r="B49">
         <v>8</v>
@@ -983,9 +1425,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>14125</v>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>58</v>
       </c>
       <c r="B50">
         <v>10</v>
@@ -994,9 +1436,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>14126</v>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>59</v>
       </c>
       <c r="B51">
         <v>10</v>
@@ -1005,17 +1447,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>14127</v>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>60</v>
       </c>
       <c r="B52">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>14128</v>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>61</v>
       </c>
       <c r="B53">
         <v>10</v>
@@ -1024,17 +1466,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>14129</v>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>62</v>
       </c>
       <c r="B54">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>14130</v>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>63</v>
       </c>
       <c r="B55">
         <v>9</v>
@@ -1043,9 +1485,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>14131</v>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>64</v>
       </c>
       <c r="B56">
         <v>10</v>
@@ -1054,9 +1496,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>14132</v>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>65</v>
       </c>
       <c r="B57">
         <v>9</v>
@@ -1065,17 +1507,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>14133</v>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>66</v>
       </c>
       <c r="B58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>14134</v>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>67</v>
       </c>
       <c r="B59">
         <v>10</v>
@@ -1084,9 +1526,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>14135</v>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>68</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -1095,57 +1537,57 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>14136</v>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>69</v>
       </c>
       <c r="B61">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>14137</v>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>70</v>
       </c>
       <c r="B62">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>14138</v>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>71</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>14139</v>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>72</v>
       </c>
       <c r="B64">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>14140</v>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>73</v>
       </c>
       <c r="B65">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>14141</v>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>74</v>
       </c>
       <c r="B66">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>14142</v>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>75</v>
       </c>
       <c r="B67">
         <v>10</v>
@@ -1154,17 +1596,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>14143</v>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>76</v>
       </c>
       <c r="B68">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>14144</v>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>77</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -1173,17 +1615,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>14145</v>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>78</v>
       </c>
       <c r="B70">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>14146</v>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>79</v>
       </c>
       <c r="B71">
         <v>9</v>
@@ -1192,9 +1634,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>14147</v>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>80</v>
       </c>
       <c r="B72">
         <v>9</v>
@@ -1203,9 +1645,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>14148</v>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>81</v>
       </c>
       <c r="B73">
         <v>10</v>
@@ -1214,9 +1656,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>14149</v>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>82</v>
       </c>
       <c r="B74">
         <v>10</v>
@@ -1225,9 +1667,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>14290</v>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>83</v>
       </c>
       <c r="B75">
         <v>9</v>
@@ -1236,9 +1678,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>14291</v>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>84</v>
       </c>
       <c r="B76">
         <v>9</v>
@@ -1247,9 +1689,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>14292</v>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>85</v>
       </c>
       <c r="B77">
         <v>9</v>
@@ -1258,20 +1700,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>14293</v>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>86</v>
       </c>
       <c r="B78">
         <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>14294</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>87</v>
       </c>
       <c r="B79">
         <v>8</v>
@@ -1280,9 +1722,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>14295</v>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>88</v>
       </c>
       <c r="B80">
         <v>6</v>
@@ -1291,9 +1733,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>14296</v>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>89</v>
       </c>
       <c r="B81">
         <v>10</v>
@@ -1302,9 +1744,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>14297</v>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>90</v>
       </c>
       <c r="B82">
         <v>6</v>
@@ -1313,9 +1755,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>14298</v>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>91</v>
       </c>
       <c r="B83">
         <v>10</v>
@@ -1324,9 +1766,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>14299</v>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>92</v>
       </c>
       <c r="B84">
         <v>9</v>
@@ -1335,9 +1777,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>14300</v>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>93</v>
       </c>
       <c r="B85">
         <v>9</v>
@@ -1349,12 +1791,12 @@
         <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <v>14301</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>94</v>
       </c>
       <c r="B86">
         <v>10</v>
@@ -1363,9 +1805,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <v>14302</v>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>95</v>
       </c>
       <c r="B87">
         <v>8</v>
@@ -1377,9 +1819,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <v>14303</v>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>96</v>
       </c>
       <c r="B88">
         <v>9</v>
@@ -1388,9 +1830,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <v>14304</v>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>97</v>
       </c>
       <c r="B89">
         <v>9</v>
@@ -1399,17 +1841,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>14305</v>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>98</v>
       </c>
       <c r="B90">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <v>14306</v>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>99</v>
       </c>
       <c r="B91">
         <v>10</v>
@@ -1418,17 +1860,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>14307</v>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>100</v>
       </c>
       <c r="B92">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>14308</v>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>101</v>
       </c>
       <c r="B93">
         <v>9</v>
@@ -1437,9 +1879,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>14309</v>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>102</v>
       </c>
       <c r="B94">
         <v>9</v>
@@ -1448,17 +1890,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>14310</v>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>103</v>
       </c>
       <c r="B95">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>14311</v>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>104</v>
       </c>
       <c r="B96">
         <v>10</v>
@@ -1467,9 +1909,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>14312</v>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>105</v>
       </c>
       <c r="B97">
         <v>9</v>
@@ -1478,9 +1920,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>14313</v>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>106</v>
       </c>
       <c r="B98">
         <v>9</v>
@@ -1489,9 +1931,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>14314</v>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>107</v>
       </c>
       <c r="B99">
         <v>8</v>
@@ -1500,9 +1942,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>14315</v>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>108</v>
       </c>
       <c r="B100">
         <v>10</v>
@@ -1511,41 +1953,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>14394</v>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>109</v>
       </c>
       <c r="B101">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>14395</v>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>110</v>
       </c>
       <c r="B102">
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>14396</v>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>111</v>
       </c>
       <c r="B103">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>14397</v>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>112</v>
       </c>
       <c r="B104">
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>14398</v>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>113</v>
       </c>
       <c r="B105">
         <v>9</v>
@@ -1557,9 +1999,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>14399</v>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>114</v>
       </c>
       <c r="B106">
         <v>9</v>
@@ -1568,9 +2010,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>14400</v>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>115</v>
       </c>
       <c r="B107">
         <v>10</v>
@@ -1582,20 +2024,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>14401</v>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>116</v>
       </c>
       <c r="B108">
         <v>7</v>
       </c>
       <c r="F108" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>14402</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>117</v>
       </c>
       <c r="B109">
         <v>9</v>
@@ -1604,9 +2046,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>14403</v>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>118</v>
       </c>
       <c r="B110">
         <v>10</v>
@@ -1618,9 +2060,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <v>14404</v>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>119</v>
       </c>
       <c r="B111">
         <v>9</v>
@@ -1632,9 +2074,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <v>14405</v>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>120</v>
       </c>
       <c r="B112">
         <v>10</v>
@@ -1643,17 +2085,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <v>14406</v>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>121</v>
       </c>
       <c r="B113">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <v>14407</v>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>122</v>
       </c>
       <c r="B114">
         <v>9</v>
@@ -1662,9 +2104,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <v>14408</v>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>123</v>
       </c>
       <c r="B115">
         <v>9</v>
@@ -1673,25 +2115,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <v>14409</v>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>124</v>
       </c>
       <c r="B116">
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <v>14410</v>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>125</v>
       </c>
       <c r="B117">
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <v>14411</v>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>126</v>
       </c>
       <c r="B118">
         <v>9</v>
@@ -1700,44 +2142,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>14412</v>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>127</v>
       </c>
       <c r="B119">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <v>14413</v>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>128</v>
       </c>
       <c r="B120">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <v>14414</v>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>129</v>
       </c>
       <c r="B121">
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <v>14415</v>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>130</v>
       </c>
       <c r="B122">
         <v>10</v>
       </c>
       <c r="F122" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <v>14416</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>131</v>
       </c>
       <c r="B123">
         <v>10</v>
@@ -1746,17 +2188,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <v>14417</v>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>132</v>
       </c>
       <c r="B124">
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <v>14418</v>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>133</v>
       </c>
       <c r="B125">
         <v>8</v>
@@ -1765,9 +2207,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <v>14419</v>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>134</v>
       </c>
       <c r="B126">
         <v>9</v>
@@ -1776,9 +2218,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <v>14420</v>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>135</v>
       </c>
       <c r="B127">
         <v>7</v>
@@ -1787,9 +2229,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <v>14421</v>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>136</v>
       </c>
       <c r="B128">
         <v>7</v>
@@ -1801,17 +2243,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <v>14422</v>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>137</v>
       </c>
       <c r="B129">
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <v>14423</v>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>138</v>
       </c>
       <c r="B130">
         <v>9</v>
@@ -1820,9 +2262,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <v>14424</v>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>139</v>
       </c>
       <c r="B131">
         <v>8</v>
@@ -1831,9 +2273,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A132">
-        <v>14425</v>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>140</v>
       </c>
       <c r="B132">
         <v>8</v>
@@ -1848,9 +2290,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A133">
-        <v>14426</v>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>141</v>
       </c>
       <c r="B133">
         <v>7</v>
@@ -1859,17 +2301,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134">
-        <v>14427</v>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>142</v>
       </c>
       <c r="B134">
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135">
-        <v>14428</v>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>143</v>
       </c>
       <c r="B135">
         <v>9</v>
@@ -1878,9 +2320,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136">
-        <v>14429</v>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>144</v>
       </c>
       <c r="B136">
         <v>9</v>
@@ -1889,9 +2331,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137">
-        <v>14430</v>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>145</v>
       </c>
       <c r="B137">
         <v>7</v>
@@ -1900,9 +2342,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A138">
-        <v>14431</v>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>146</v>
       </c>
       <c r="B138">
         <v>10</v>
@@ -1914,9 +2356,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A139">
-        <v>14432</v>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>147</v>
       </c>
       <c r="B139">
         <v>9</v>
@@ -1925,9 +2367,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A140">
-        <v>14433</v>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>148</v>
       </c>
       <c r="B140">
         <v>6</v>
@@ -1936,9 +2378,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A141">
-        <v>14434</v>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>149</v>
       </c>
       <c r="B141">
         <v>8</v>
@@ -1947,9 +2389,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A142">
-        <v>14435</v>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>150</v>
       </c>
       <c r="B142">
         <v>7</v>
@@ -1958,9 +2400,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143">
-        <v>14436</v>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>151</v>
       </c>
       <c r="B143">
         <v>8</v>
@@ -1969,9 +2411,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A144">
-        <v>14437</v>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>152</v>
       </c>
       <c r="B144">
         <v>10</v>
@@ -1980,9 +2422,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145">
-        <v>14438</v>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>153</v>
       </c>
       <c r="B145">
         <v>9</v>
@@ -1991,9 +2433,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146">
-        <v>14439</v>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>154</v>
       </c>
       <c r="B146">
         <v>10</v>

</xml_diff>